<commit_message>
complete raw data from Galot
</commit_message>
<xml_diff>
--- a/Telemetry/Galot/notes_2019-06-07.xlsx
+++ b/Telemetry/Galot/notes_2019-06-07.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>Galot Data Log</t>
   </si>
@@ -162,6 +162,48 @@
   </si>
   <si>
     <t>Motor controller is running tag delay_duty</t>
+  </si>
+  <si>
+    <t>test1.TXT</t>
+  </si>
+  <si>
+    <t>Cornering test</t>
+  </si>
+  <si>
+    <t>CW</t>
+  </si>
+  <si>
+    <t>CCW</t>
+  </si>
+  <si>
+    <t>30m radius, CCW</t>
+  </si>
+  <si>
+    <t>accelerate to speed then spindown in a circle</t>
+  </si>
+  <si>
+    <t>Run 3</t>
+  </si>
+  <si>
+    <t>Run 4</t>
+  </si>
+  <si>
+    <t>30m radius, CW</t>
+  </si>
+  <si>
+    <t>cornering1.TXT</t>
+  </si>
+  <si>
+    <t>race sim</t>
+  </si>
+  <si>
+    <t>full 7 laps</t>
+  </si>
+  <si>
+    <t>flying start</t>
+  </si>
+  <si>
+    <t>racesim2.TXT</t>
   </si>
 </sst>
 </file>
@@ -219,11 +261,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,6 +797,9 @@
       <c r="C22" t="s">
         <v>33</v>
       </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
       <c r="E22">
         <v>680</v>
       </c>
@@ -768,6 +814,9 @@
       <c r="C23" t="s">
         <v>35</v>
       </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
       <c r="E23">
         <v>690</v>
       </c>
@@ -794,6 +843,110 @@
       </c>
       <c r="C26" t="s">
         <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final raw data from Galot
</commit_message>
<xml_diff>
--- a/Telemetry/Galot/notes_2019-06-07.xlsx
+++ b/Telemetry/Galot/notes_2019-06-07.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
   <si>
     <t>Galot Data Log</t>
   </si>
@@ -204,6 +204,27 @@
   </si>
   <si>
     <t>racesim2.TXT</t>
+  </si>
+  <si>
+    <t>spindown @ 10m/s</t>
+  </si>
+  <si>
+    <t>downhill</t>
+  </si>
+  <si>
+    <t>uphill</t>
+  </si>
+  <si>
+    <t>along the wider section of the road</t>
+  </si>
+  <si>
+    <t>spindowns5.TXT</t>
+  </si>
+  <si>
+    <t>spindown on sticky</t>
+  </si>
+  <si>
+    <t>TIRE POPPED AT END</t>
   </si>
 </sst>
 </file>
@@ -544,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -949,6 +970,61 @@
         <v>54</v>
       </c>
     </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" t="s">
+        <v>59</v>
+      </c>
+      <c r="H38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>